<commit_message>
I guess ill try and godot
</commit_message>
<xml_diff>
--- a/OneArmedBandits/Payouts.xlsx
+++ b/OneArmedBandits/Payouts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thorb\source\repos\MonteCarlo\OneArmedBandits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEDD507-9AD5-4AC8-AB8F-527A6187B5C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76C85C3-E3D6-47D8-93DF-703A2BC3FBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8BC131A-8BAF-4A72-8A95-4E33A6F95728}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8BC131A-8BAF-4A72-8A95-4E33A6F95728}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
+    <sheet name="Wild 0s" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Symbols</t>
   </si>
@@ -47,26 +48,31 @@
     <t>Chance</t>
   </si>
   <si>
-    <t>EV</t>
-  </si>
-  <si>
     <t>Payout</t>
   </si>
   <si>
     <t>bet</t>
   </si>
   <si>
-    <t>PAYOUT</t>
+    <t>Payout increase per hit</t>
+  </si>
+  <si>
+    <t>Per spin payout</t>
+  </si>
+  <si>
+    <t>Occurence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.000\ _k_r_._-;\-* #,##0.000\ _k_r_._-;_-* &quot;-&quot;???\ _k_r_._-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -186,11 +192,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -199,10 +205,10 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -211,15 +217,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -536,13 +543,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F6F985-3E21-42CC-B310-25DE97E9EA14}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C27" sqref="C27:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
@@ -587,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -749,47 +761,47 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6">
         <f>((C1+1)*$B$10)*$B$6</f>
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:L6" si="3">((D1+1)*$B$10)*$B$6</f>
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>1050</v>
+        <v>1200</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>1750</v>
+        <v>2000</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>2450</v>
+        <v>2800</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>2800</v>
+        <v>3200</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>3150</v>
+        <v>3600</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="2"/>
@@ -855,7 +867,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -870,8 +882,8 @@
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
-        <v>3</v>
+      <c r="B13" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="O13" s="11"/>
     </row>
@@ -916,201 +928,176 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="14">
-        <f>SUM(C14:L14)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C15" s="13">
-        <f t="shared" ref="C15:K18" si="6">(C4*$N4)-(C14*$N$3)</f>
-        <v>5.000000000000001E-2</v>
-      </c>
-      <c r="D15" s="13">
+      <c r="C15" s="15">
+        <f>C4-C3</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" ref="D15:L15" si="6">D4-D3</f>
+        <v>10</v>
+      </c>
+      <c r="E15" s="15">
         <f t="shared" si="6"/>
-        <v>0.10000000000000002</v>
-      </c>
-      <c r="E15" s="13">
+        <v>15</v>
+      </c>
+      <c r="F15" s="15">
         <f t="shared" si="6"/>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="F15" s="13">
+        <v>20</v>
+      </c>
+      <c r="G15" s="15">
         <f t="shared" si="6"/>
-        <v>0.20000000000000004</v>
-      </c>
-      <c r="G15" s="13">
+        <v>25</v>
+      </c>
+      <c r="H15" s="15">
         <f t="shared" si="6"/>
-        <v>0.25000000000000006</v>
-      </c>
-      <c r="H15" s="13">
+        <v>30</v>
+      </c>
+      <c r="I15" s="15">
         <f t="shared" si="6"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="I15" s="13">
+        <v>35</v>
+      </c>
+      <c r="J15" s="15">
         <f t="shared" si="6"/>
-        <v>0.35000000000000009</v>
-      </c>
-      <c r="J15" s="13">
+        <v>40</v>
+      </c>
+      <c r="K15" s="15">
         <f t="shared" si="6"/>
-        <v>0.40000000000000008</v>
-      </c>
-      <c r="K15" s="13">
+        <v>45</v>
+      </c>
+      <c r="L15" s="15">
         <f t="shared" si="6"/>
-        <v>0.45000000000000007</v>
-      </c>
-      <c r="L15" s="13">
-        <f>(L4*$N4)-(L14*$N$3)</f>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="14">
-        <f t="shared" ref="N15:N18" si="7">SUM(C15:L15)</f>
-        <v>2.7500000000000004</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C16" s="13">
-        <f t="shared" si="6"/>
-        <v>9.5000000000000015E-2</v>
-      </c>
-      <c r="D16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.19000000000000003</v>
-      </c>
-      <c r="E16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.28500000000000003</v>
-      </c>
-      <c r="F16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.38000000000000006</v>
-      </c>
-      <c r="G16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.47500000000000009</v>
-      </c>
-      <c r="H16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="I16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.66500000000000015</v>
-      </c>
-      <c r="J16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.76000000000000012</v>
-      </c>
-      <c r="K16" s="13">
-        <f t="shared" si="6"/>
-        <v>0.8550000000000002</v>
-      </c>
-      <c r="L16" s="13">
-        <f t="shared" ref="L16:L18" si="8">(L5*$N5)-(L15*$N$3)</f>
-        <v>0.95000000000000018</v>
-      </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="14">
-        <f t="shared" si="7"/>
-        <v>5.2250000000000014</v>
-      </c>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C17" s="13">
-        <f t="shared" si="6"/>
-        <v>2.5500000000000009E-2</v>
-      </c>
-      <c r="D17" s="13">
-        <f t="shared" si="6"/>
-        <v>5.1000000000000018E-2</v>
-      </c>
-      <c r="E17" s="13">
-        <f t="shared" si="6"/>
-        <v>7.650000000000004E-2</v>
-      </c>
-      <c r="F17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.10200000000000004</v>
-      </c>
-      <c r="G17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.12750000000000003</v>
-      </c>
-      <c r="H17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.15300000000000008</v>
-      </c>
-      <c r="I17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.17850000000000005</v>
-      </c>
-      <c r="J17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.20400000000000007</v>
-      </c>
-      <c r="K17" s="13">
-        <f t="shared" si="6"/>
-        <v>0.22950000000000009</v>
-      </c>
-      <c r="L17" s="13">
-        <f t="shared" si="8"/>
-        <v>0.25500000000000006</v>
-      </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="14">
-        <f t="shared" si="7"/>
-        <v>1.4025000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="13">
-        <f t="shared" si="6"/>
-        <v>7.4500000000000026E-3</v>
-      </c>
-      <c r="D18" s="13">
-        <f t="shared" si="6"/>
-        <v>1.4900000000000005E-2</v>
-      </c>
-      <c r="E18" s="13">
-        <f t="shared" si="6"/>
-        <v>2.2350000000000009E-2</v>
-      </c>
-      <c r="F18" s="13">
-        <f t="shared" si="6"/>
-        <v>2.9800000000000011E-2</v>
-      </c>
-      <c r="G18" s="13">
-        <f t="shared" si="6"/>
-        <v>3.7250000000000019E-2</v>
-      </c>
-      <c r="H18" s="13">
-        <f t="shared" si="6"/>
-        <v>4.4700000000000017E-2</v>
-      </c>
-      <c r="I18" s="13">
-        <f t="shared" si="6"/>
-        <v>5.215000000000003E-2</v>
-      </c>
-      <c r="J18" s="13">
-        <f t="shared" si="6"/>
-        <v>5.9600000000000021E-2</v>
-      </c>
-      <c r="K18" s="13">
-        <f t="shared" si="6"/>
-        <v>6.7050000000000026E-2</v>
-      </c>
-      <c r="L18" s="13">
-        <f t="shared" si="8"/>
-        <v>7.4500000000000038E-2</v>
-      </c>
-      <c r="M18" s="1"/>
-      <c r="N18" s="15">
-        <f t="shared" si="7"/>
-        <v>0.40975000000000017</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="15">
+        <f t="shared" ref="C16:L18" si="7">C5-C4</f>
+        <v>95</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="7"/>
+        <v>190</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="7"/>
+        <v>285</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="7"/>
+        <v>380</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="7"/>
+        <v>475</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="7"/>
+        <v>570</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="7"/>
+        <v>665</v>
+      </c>
+      <c r="J16" s="15">
+        <f t="shared" si="7"/>
+        <v>760</v>
+      </c>
+      <c r="K16" s="15">
+        <f t="shared" si="7"/>
+        <v>855</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="7"/>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="15">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="7"/>
+        <v>900</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="7"/>
+        <v>1200</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="7"/>
+        <v>1500</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="7"/>
+        <v>1800</v>
+      </c>
+      <c r="I17" s="15">
+        <f t="shared" si="7"/>
+        <v>2100</v>
+      </c>
+      <c r="J17" s="15">
+        <f t="shared" si="7"/>
+        <v>2400</v>
+      </c>
+      <c r="K17" s="15">
+        <f t="shared" si="7"/>
+        <v>2700</v>
+      </c>
+      <c r="L17" s="15">
+        <f t="shared" si="7"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="15">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="7"/>
+        <v>1200</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="7"/>
+        <v>1800</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="7"/>
+        <v>2400</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="7"/>
+        <v>3000</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="7"/>
+        <v>3600</v>
+      </c>
+      <c r="I18" s="15">
+        <f t="shared" si="7"/>
+        <v>4200</v>
+      </c>
+      <c r="J18" s="15">
+        <f t="shared" si="7"/>
+        <v>4800</v>
+      </c>
+      <c r="K18" s="15">
+        <f t="shared" si="7"/>
+        <v>5400</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="7"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1121,12 +1108,1118 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="1" t="s">
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="17">
-        <f>(SUM(N14:N18)/B10)</f>
-        <v>0.97872500000000018</v>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C22" s="16">
+        <f>C14*$N3</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" ref="D22:L22" si="8">D14*$N3</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L22" s="16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="16">
+        <f>SUM(C22:L22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="16">
+        <f t="shared" ref="C23:L26" si="9">C15*$N4</f>
+        <v>5.000000000000001E-2</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="E23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="G23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="H23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="I23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="J23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="K23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="L23" s="16">
+        <f t="shared" si="9"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="N23" s="16">
+        <f t="shared" ref="N23:N26" si="10">SUM(C23:L23)</f>
+        <v>2.7500000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C24" s="16">
+        <f t="shared" si="9"/>
+        <v>9.5000000000000029E-2</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.19000000000000006</v>
+      </c>
+      <c r="E24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.28500000000000009</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.38000000000000012</v>
+      </c>
+      <c r="G24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.47500000000000009</v>
+      </c>
+      <c r="H24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.57000000000000017</v>
+      </c>
+      <c r="I24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.66500000000000015</v>
+      </c>
+      <c r="J24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.76000000000000023</v>
+      </c>
+      <c r="K24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.8550000000000002</v>
+      </c>
+      <c r="L24" s="16">
+        <f t="shared" si="9"/>
+        <v>0.95000000000000018</v>
+      </c>
+      <c r="N24" s="16">
+        <f t="shared" si="10"/>
+        <v>5.2250000000000014</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="16">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000009E-2</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="9"/>
+        <v>6.0000000000000019E-2</v>
+      </c>
+      <c r="E25" s="16">
+        <f t="shared" si="9"/>
+        <v>9.0000000000000024E-2</v>
+      </c>
+      <c r="F25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.12000000000000004</v>
+      </c>
+      <c r="G25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.15000000000000005</v>
+      </c>
+      <c r="H25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.18000000000000005</v>
+      </c>
+      <c r="I25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.21000000000000008</v>
+      </c>
+      <c r="J25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="K25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.27000000000000007</v>
+      </c>
+      <c r="L25" s="16">
+        <f t="shared" si="9"/>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="N25" s="16">
+        <f t="shared" si="10"/>
+        <v>1.6500000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="17">
+        <f t="shared" si="9"/>
+        <v>6.0000000000000027E-3</v>
+      </c>
+      <c r="D26" s="17">
+        <f t="shared" si="9"/>
+        <v>1.2000000000000005E-2</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="9"/>
+        <v>1.8000000000000009E-2</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="9"/>
+        <v>2.4000000000000011E-2</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="9"/>
+        <v>3.0000000000000013E-2</v>
+      </c>
+      <c r="H26" s="17">
+        <f t="shared" si="9"/>
+        <v>3.6000000000000018E-2</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" si="9"/>
+        <v>4.2000000000000016E-2</v>
+      </c>
+      <c r="J26" s="17">
+        <f t="shared" si="9"/>
+        <v>4.8000000000000022E-2</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="9"/>
+        <v>5.400000000000002E-2</v>
+      </c>
+      <c r="L26" s="17">
+        <f t="shared" si="9"/>
+        <v>6.0000000000000026E-2</v>
+      </c>
+      <c r="N26" s="17">
+        <f t="shared" si="10"/>
+        <v>0.33000000000000018</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C27" s="16">
+        <f>SUM(C22:C26)</f>
+        <v>0.18100000000000005</v>
+      </c>
+      <c r="D27" s="16">
+        <f t="shared" ref="D27:L27" si="11">SUM(D22:D26)</f>
+        <v>0.3620000000000001</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" si="11"/>
+        <v>0.54300000000000015</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="11"/>
+        <v>0.7240000000000002</v>
+      </c>
+      <c r="G27" s="16">
+        <f t="shared" si="11"/>
+        <v>0.90500000000000014</v>
+      </c>
+      <c r="H27" s="16">
+        <f t="shared" si="11"/>
+        <v>1.0860000000000003</v>
+      </c>
+      <c r="I27" s="16">
+        <f t="shared" si="11"/>
+        <v>1.2670000000000001</v>
+      </c>
+      <c r="J27" s="16">
+        <f t="shared" si="11"/>
+        <v>1.4480000000000004</v>
+      </c>
+      <c r="K27" s="16">
+        <f t="shared" si="11"/>
+        <v>1.6290000000000002</v>
+      </c>
+      <c r="L27" s="16">
+        <f t="shared" si="11"/>
+        <v>1.8100000000000003</v>
+      </c>
+      <c r="N27" s="1">
+        <f>SUM(N22:N26)/B10</f>
+        <v>0.99550000000000016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00134590-22A3-4566-B749-0E053ADB17B9}">
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10">
+        <v>3</v>
+      </c>
+      <c r="G1" s="10">
+        <v>4</v>
+      </c>
+      <c r="H1" s="10">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10">
+        <v>6</v>
+      </c>
+      <c r="J1" s="10">
+        <v>7</v>
+      </c>
+      <c r="K1" s="10">
+        <v>8</v>
+      </c>
+      <c r="L1" s="10">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="O3" s="2">
+        <f>N3</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <f>($B$10)*$B$4</f>
+        <v>2.5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:L4" si="0">((D1+1)*$B$10)*$B$4</f>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="N4">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="O4" s="2">
+        <f>O3*N4</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <f>($B$10)*$B$5</f>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:L5" si="1">((D1+1)*$B$10)*$B$5</f>
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N7" si="2">2/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O7" si="3">O4*N5</f>
+        <v>8.0000000000000019E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>($B$10)*$B$6</f>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:L6" si="4">((D1+1)*$B$10)*$B$6</f>
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6000000000000005E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="18">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <f>($B$10)*$B$7</f>
+        <v>150</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:L7" si="5">((D1+1)*$B$10)*$B$7</f>
+        <v>300</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="5"/>
+        <v>450</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="5"/>
+        <v>600</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="5"/>
+        <v>750</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>900</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>1050</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>1200</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>1350</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="5"/>
+        <v>1500</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2000000000000013E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="11"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="O10" s="11"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="12"/>
+      <c r="O11" s="11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="11"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="13">
+        <f>(C3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
+        <f>(D3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <f>(E3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <f>(F3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <f>(G3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <f>(H3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <f>(I3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <f>(J3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <f>(K3*$O3)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="13">
+        <f>(L3*$O3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="15">
+        <f>C4-C3</f>
+        <v>2.5</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" ref="D15:L15" si="6">D4-D3</f>
+        <v>5</v>
+      </c>
+      <c r="E15" s="15">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+      <c r="F15" s="15">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" si="6"/>
+        <v>12.5</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="I15" s="15">
+        <f t="shared" si="6"/>
+        <v>17.5</v>
+      </c>
+      <c r="J15" s="15">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="K15" s="15">
+        <f t="shared" si="6"/>
+        <v>22.5</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="15">
+        <f t="shared" ref="C16:L18" si="7">C5-C4</f>
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="7"/>
+        <v>7.5</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="7"/>
+        <v>12.5</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="7"/>
+        <v>17.5</v>
+      </c>
+      <c r="J16" s="15">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="K16" s="15">
+        <f t="shared" si="7"/>
+        <v>22.5</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="F17" s="15">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="I17" s="15">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="J17" s="15">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="K17" s="15">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="L17" s="15">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="15">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="7"/>
+        <v>280</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="7"/>
+        <v>420</v>
+      </c>
+      <c r="F18" s="15">
+        <f t="shared" si="7"/>
+        <v>560</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="7"/>
+        <v>700</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="7"/>
+        <v>840</v>
+      </c>
+      <c r="I18" s="15">
+        <f t="shared" si="7"/>
+        <v>980</v>
+      </c>
+      <c r="J18" s="15">
+        <f t="shared" si="7"/>
+        <v>1120</v>
+      </c>
+      <c r="K18" s="15">
+        <f t="shared" si="7"/>
+        <v>1260</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="7"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C22" s="16">
+        <f>C14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="16">
+        <f>D14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="16">
+        <f>E14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="16">
+        <f>F14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="16">
+        <f>G14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <f>H14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
+        <f>I14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="16">
+        <f>J14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="16">
+        <f>K14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="16">
+        <f>L14*$O3</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="16">
+        <f>SUM(C22:L22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C23" s="16">
+        <f>C15*$O4</f>
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="D23" s="16">
+        <f>D15*$O4</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="E23" s="16">
+        <f>E15*$O4</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F23" s="16">
+        <f>F15*$O4</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="G23" s="16">
+        <f>G15*$O4</f>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="H23" s="16">
+        <f>H15*$O4</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I23" s="16">
+        <f>I15*$O4</f>
+        <v>0.70000000000000018</v>
+      </c>
+      <c r="J23" s="16">
+        <f>J15*$O4</f>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="K23" s="16">
+        <f>K15*$O4</f>
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="L23" s="16">
+        <f>L15*$O4</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="N23" s="16">
+        <f t="shared" ref="N23:N26" si="8">SUM(C23:L23)</f>
+        <v>5.5000000000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C24" s="16">
+        <f>C16*$O5</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D24" s="16">
+        <f>D16*$O5</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E24" s="16">
+        <f>E16*$O5</f>
+        <v>6.0000000000000012E-2</v>
+      </c>
+      <c r="F24" s="16">
+        <f>F16*$O5</f>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="G24" s="16">
+        <f>G16*$O5</f>
+        <v>0.10000000000000002</v>
+      </c>
+      <c r="H24" s="16">
+        <f>H16*$O5</f>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="I24" s="16">
+        <f>I16*$O5</f>
+        <v>0.14000000000000004</v>
+      </c>
+      <c r="J24" s="16">
+        <f>J16*$O5</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="K24" s="16">
+        <f>K16*$O5</f>
+        <v>0.18000000000000005</v>
+      </c>
+      <c r="L24" s="16">
+        <f>L16*$O5</f>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="N24" s="16">
+        <f t="shared" si="8"/>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C25" s="16">
+        <f>C17*$O6</f>
+        <v>8.0000000000000019E-3</v>
+      </c>
+      <c r="D25" s="16">
+        <f>D17*$O6</f>
+        <v>1.6000000000000004E-2</v>
+      </c>
+      <c r="E25" s="16">
+        <f>E17*$O6</f>
+        <v>2.4000000000000007E-2</v>
+      </c>
+      <c r="F25" s="16">
+        <f>F17*$O6</f>
+        <v>3.2000000000000008E-2</v>
+      </c>
+      <c r="G25" s="16">
+        <f>G17*$O6</f>
+        <v>4.0000000000000015E-2</v>
+      </c>
+      <c r="H25" s="16">
+        <f>H17*$O6</f>
+        <v>4.8000000000000015E-2</v>
+      </c>
+      <c r="I25" s="16">
+        <f>I17*$O6</f>
+        <v>5.6000000000000015E-2</v>
+      </c>
+      <c r="J25" s="16">
+        <f>J17*$O6</f>
+        <v>6.4000000000000015E-2</v>
+      </c>
+      <c r="K25" s="16">
+        <f>K17*$O6</f>
+        <v>7.2000000000000022E-2</v>
+      </c>
+      <c r="L25" s="16">
+        <f>L17*$O6</f>
+        <v>8.0000000000000029E-2</v>
+      </c>
+      <c r="N25" s="16">
+        <f t="shared" si="8"/>
+        <v>0.44000000000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C26" s="16">
+        <f>C18*$O7</f>
+        <v>4.480000000000002E-2</v>
+      </c>
+      <c r="D26" s="16">
+        <f>D18*$O7</f>
+        <v>8.9600000000000041E-2</v>
+      </c>
+      <c r="E26" s="16">
+        <f>E18*$O7</f>
+        <v>0.13440000000000005</v>
+      </c>
+      <c r="F26" s="16">
+        <f>F18*$O7</f>
+        <v>0.17920000000000008</v>
+      </c>
+      <c r="G26" s="16">
+        <f>G18*$O7</f>
+        <v>0.22400000000000009</v>
+      </c>
+      <c r="H26" s="16">
+        <f>H18*$O7</f>
+        <v>0.26880000000000009</v>
+      </c>
+      <c r="I26" s="16">
+        <f>I18*$O7</f>
+        <v>0.31360000000000016</v>
+      </c>
+      <c r="J26" s="16">
+        <f>J18*$O7</f>
+        <v>0.35840000000000016</v>
+      </c>
+      <c r="K26" s="16">
+        <f>K18*$O7</f>
+        <v>0.40320000000000017</v>
+      </c>
+      <c r="L26" s="16">
+        <f>L18*$O7</f>
+        <v>0.44800000000000018</v>
+      </c>
+      <c r="N26" s="17">
+        <f t="shared" si="8"/>
+        <v>2.4640000000000013</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="1">
+        <f>SUM(N22:N26)/B10</f>
+        <v>0.95040000000000036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>